<commit_message>
create procedure(mysql,postgre,oracle) & create mongo index
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/코드.xlsx
+++ b/DOC/1. 개발 문서/코드.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562696D6-D0B9-4AF4-8508-10D424312D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66585652-994B-4DFE-B6A2-428E82EFB783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9880" yWindow="1310" windowWidth="19200" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2480" yWindow="1980" windowWidth="19200" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
rdg / fe / BE update
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/코드.xlsx
+++ b/DOC/1. 개발 문서/코드.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66585652-994B-4DFE-B6A2-428E82EFB783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF16B30-1723-4D93-94F8-59367FE6AD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1980" windowWidth="19200" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>account</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,9 +159,6 @@
   <si>
     <t>역분개</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FAILED</t>
   </si>
   <si>
     <t>실패(잔액부족)</t>
@@ -928,7 +925,7 @@
   <dimension ref="D1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1114,10 +1111,10 @@
         <v>5</v>
       </c>
       <c r="G14" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="27" t="s">
         <v>36</v>
-      </c>
-      <c r="H14" s="27" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="4:8" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -1130,7 +1127,7 @@
         <v>34</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="4:8" x14ac:dyDescent="0.45">
@@ -1183,7 +1180,7 @@
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.45">
       <c r="D20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>33</v>
@@ -1192,10 +1189,10 @@
         <v>1</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.45">
@@ -1205,10 +1202,10 @@
         <v>2</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.45">
@@ -1218,10 +1215,10 @@
         <v>3</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.45">
@@ -1390,7 +1387,7 @@
     <mergeCell ref="D2:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E4:H6 E7:F7 H7 E8:H9 E10:F11 H10:H11 D19:H45 E12:H18 D4:D43">
+  <conditionalFormatting sqref="E4:H6 D4:D43 E7:F7 H7 E8:H9 E10:F11 H10:H11 E12:H18 D19:H45">
     <cfRule type="expression" dxfId="0" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>